<commit_message>
mboh lali update opo
</commit_message>
<xml_diff>
--- a/Revisi Anggaran/17 Maret 2023/2c. Revisi MK 2023.xlsx
+++ b/Revisi Anggaran/17 Maret 2023/2c. Revisi MK 2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\!RIA\! KEGIATAN 2023\REVISI 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACK\PUSDIK\2023\Github\TA.2023\Revisi Anggaran\17 Maret 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57C5314-8CDA-43D5-9EF2-EE70134A533D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D8634C-4972-467B-BEC0-026174239ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{565EA5FA-1DAB-427E-93A3-16D88B5F5D47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{565EA5FA-1DAB-427E-93A3-16D88B5F5D47}"/>
   </bookViews>
   <sheets>
     <sheet name="USULAN REVISI" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1043,6 +1054,39 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1061,38 +1105,26 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1102,27 +1134,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1458,112 +1469,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD0258F-BBF2-4E29-BA1E-8CC0129EFF16}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="6" style="13" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="14" style="13" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="52.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="1.109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="52.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" style="13" customWidth="1"/>
     <col min="11" max="11" width="7" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="13" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="13" customWidth="1"/>
-    <col min="14" max="15" width="11.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="13" customWidth="1"/>
+    <col min="14" max="15" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="115" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-    </row>
-    <row r="2" spans="1:16" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="115" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-    </row>
-    <row r="3" spans="1:16" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="116"/>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-    </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="118"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-    </row>
-    <row r="5" spans="1:16" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+    </row>
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="110"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+    </row>
+    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="112"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+    </row>
+    <row r="5" spans="1:16" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="121"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="115"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="125" t="s">
+      <c r="H5" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="125"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="119"/>
       <c r="N5" t="s">
         <v>104</v>
       </c>
@@ -1571,91 +1582,91 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="116"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="118"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="125"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125"/>
-    </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+    </row>
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="109" t="s">
+      <c r="D7" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="120" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="111" t="s">
+      <c r="H7" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="111" t="s">
+      <c r="I7" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="109" t="s">
+      <c r="K7" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="109" t="s">
+      <c r="L7" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="109" t="s">
+      <c r="M7" s="120" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="111"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
+    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="122"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-    </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+    </row>
+    <row r="9" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="123"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
-    </row>
-    <row r="10" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+    </row>
+    <row r="10" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1694,7 +1705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -1719,7 +1730,7 @@
         <v>-370359000</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="92" t="s">
         <v>76</v>
       </c>
@@ -1748,7 +1759,7 @@
         <v>248392000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="74">
         <v>521211</v>
       </c>
@@ -1777,7 +1788,7 @@
         <v>53175000</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="78"/>
       <c r="B14" s="79" t="s">
         <v>30</v>
@@ -1815,7 +1826,7 @@
         <v>42675000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="78"/>
       <c r="B15" s="79" t="s">
         <v>31</v>
@@ -1852,7 +1863,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="78"/>
       <c r="B16" s="79" t="s">
         <v>33</v>
@@ -1889,7 +1900,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78"/>
       <c r="B17" s="79" t="s">
         <v>34</v>
@@ -1926,7 +1937,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="74">
         <v>522151</v>
       </c>
@@ -1955,7 +1966,7 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
       <c r="B19" s="79" t="s">
         <v>35</v>
@@ -1992,7 +2003,7 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="74">
         <v>524111</v>
       </c>
@@ -2021,7 +2032,7 @@
         <v>67448000</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19" t="s">
         <v>36</v>
@@ -2066,7 +2077,7 @@
         <v>56803400</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -2086,7 +2097,7 @@
         <v>111769000</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="19"/>
       <c r="C23" s="20"/>
@@ -2113,7 +2124,7 @@
         <v>83790000</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
@@ -2141,7 +2152,7 @@
         <v>27979000</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>77</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>83319000</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="74">
         <v>521211</v>
       </c>
@@ -2199,7 +2210,7 @@
         <v>36300000</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="78"/>
       <c r="B27" s="79" t="s">
         <v>30</v>
@@ -2237,7 +2248,7 @@
         <v>11550000</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="78"/>
       <c r="B28" s="79" t="s">
         <v>31</v>
@@ -2274,7 +2285,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="78"/>
       <c r="B29" s="79" t="s">
         <v>33</v>
@@ -2311,7 +2322,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78"/>
       <c r="B30" s="79" t="s">
         <v>34</v>
@@ -2348,7 +2359,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78"/>
       <c r="B31" s="79"/>
       <c r="C31" s="80"/>
@@ -2375,7 +2386,7 @@
         <v>16500000</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="74">
         <v>522151</v>
       </c>
@@ -2404,7 +2415,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="78"/>
       <c r="B33" s="79" t="s">
         <v>35</v>
@@ -2441,7 +2452,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="74">
         <v>524111</v>
       </c>
@@ -2477,7 +2488,7 @@
         <v>16119000</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="78"/>
       <c r="B35" s="79" t="s">
         <v>37</v>
@@ -2514,7 +2525,7 @@
         <v>32019000</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A36" s="93" t="s">
         <v>75</v>
       </c>
@@ -2547,7 +2558,7 @@
         <v>16500000</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>42</v>
       </c>
@@ -2577,7 +2588,7 @@
       </c>
       <c r="N37" s="105"/>
     </row>
-    <row r="38" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="28"/>
       <c r="B38" s="29" t="s">
         <v>30</v>
@@ -2616,7 +2627,7 @@
       </c>
       <c r="N38" s="105"/>
     </row>
-    <row r="39" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28"/>
       <c r="B39" s="29" t="s">
         <v>31</v>
@@ -2653,7 +2664,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="28"/>
       <c r="B40" s="29" t="s">
         <v>33</v>
@@ -2690,7 +2701,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="28"/>
       <c r="B41" s="29" t="s">
         <v>34</v>
@@ -2727,7 +2738,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>43</v>
       </c>
@@ -2756,7 +2767,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="29" t="s">
         <v>44</v>
@@ -2793,7 +2804,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
         <v>45</v>
       </c>
@@ -2822,7 +2833,7 @@
         <v>55034000</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="B45" s="29" t="s">
         <v>46</v>
@@ -2867,7 +2878,7 @@
       </c>
       <c r="P45" s="105"/>
     </row>
-    <row r="46" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="92" t="s">
         <v>74</v>
       </c>
@@ -2901,7 +2912,7 @@
       </c>
       <c r="P46" s="105"/>
     </row>
-    <row r="47" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="74">
         <v>521211</v>
       </c>
@@ -2930,7 +2941,7 @@
         <v>15500000</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="78"/>
       <c r="B48" s="79" t="s">
         <v>30</v>
@@ -2968,7 +2979,7 @@
         <v>9750000</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="78"/>
       <c r="B49" s="79" t="s">
         <v>39</v>
@@ -3005,7 +3016,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="78"/>
       <c r="B50" s="79" t="s">
         <v>33</v>
@@ -3042,7 +3053,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="78"/>
       <c r="B51" s="79" t="s">
         <v>34</v>
@@ -3079,7 +3090,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="74">
         <v>522151</v>
       </c>
@@ -3108,7 +3119,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="78"/>
       <c r="B53" s="79" t="s">
         <v>35</v>
@@ -3145,7 +3156,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="74">
         <v>524111</v>
       </c>
@@ -3174,7 +3185,7 @@
         <v>43303000</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="78"/>
       <c r="B55" s="79" t="s">
         <v>40</v>
@@ -3219,7 +3230,7 @@
       </c>
       <c r="P55" s="105"/>
     </row>
-    <row r="56" spans="1:16" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A56" s="99"/>
       <c r="B56" s="100"/>
       <c r="C56" s="99"/>
@@ -3243,7 +3254,7 @@
         <v>26887000</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="74"/>
       <c r="B57" s="75"/>
       <c r="C57" s="74"/>
@@ -3265,7 +3276,7 @@
         <v>31750000</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="78"/>
       <c r="B58" s="79"/>
       <c r="C58" s="78"/>
@@ -3291,7 +3302,7 @@
         <v>11250000</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="78"/>
       <c r="B59" s="79"/>
       <c r="C59" s="78"/>
@@ -3317,7 +3328,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="78"/>
       <c r="B60" s="79"/>
       <c r="C60" s="78"/>
@@ -3343,7 +3354,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="78"/>
       <c r="B61" s="79"/>
       <c r="C61" s="78"/>
@@ -3369,7 +3380,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="78"/>
       <c r="B62" s="79"/>
       <c r="C62" s="78"/>
@@ -3395,7 +3406,7 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="74"/>
       <c r="B63" s="75"/>
       <c r="C63" s="74"/>
@@ -3417,7 +3428,7 @@
         <v>6400000</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="78"/>
       <c r="B64" s="79"/>
       <c r="C64" s="78"/>
@@ -3443,7 +3454,7 @@
         <v>6400000</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="74"/>
       <c r="B65" s="75"/>
       <c r="C65" s="74"/>
@@ -3465,7 +3476,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="78"/>
       <c r="B66" s="79"/>
       <c r="C66" s="78"/>
@@ -3491,7 +3502,7 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="74"/>
       <c r="B67" s="75"/>
       <c r="C67" s="74"/>
@@ -3513,7 +3524,7 @@
         <v>195690000</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="78"/>
       <c r="B68" s="79"/>
       <c r="C68" s="78"/>
@@ -3539,7 +3550,7 @@
         <v>195690000</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="74"/>
       <c r="B69" s="75"/>
       <c r="C69" s="74"/>
@@ -3561,7 +3572,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="78"/>
       <c r="B70" s="79"/>
       <c r="C70" s="78"/>
@@ -3587,7 +3598,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="10"/>
       <c r="C71" s="8"/>
@@ -3602,7 +3613,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="11"/>
     </row>
-    <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="10"/>
       <c r="C72" s="8"/>
@@ -3617,7 +3628,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="11"/>
     </row>
-    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="10"/>
       <c r="C73" s="8"/>
@@ -3634,7 +3645,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="11"/>
     </row>
-    <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="102" t="s">
         <v>92</v>
@@ -3653,7 +3664,7 @@
       <c r="L74" s="8"/>
       <c r="M74" s="11"/>
     </row>
-    <row r="75" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="102" t="s">
         <v>93</v>
@@ -3671,7 +3682,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="11"/>
     </row>
-    <row r="76" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
@@ -3684,7 +3695,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="11"/>
     </row>
-    <row r="77" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="10"/>
       <c r="C77" s="8"/>
@@ -3698,7 +3709,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="10"/>
       <c r="C78" s="8"/>
@@ -3712,7 +3723,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="12" t="s">
         <v>25</v>
@@ -3728,7 +3739,7 @@
       <c r="K79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="10" t="s">
         <v>27</v>
@@ -3744,7 +3755,7 @@
       <c r="K80" s="8"/>
       <c r="M80" s="8"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3756,7 +3767,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3768,7 +3779,7 @@
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3781,7 +3792,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3794,7 +3805,7 @@
       <c r="L84" s="8"/>
       <c r="M84" s="8"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3807,7 +3818,7 @@
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3820,7 +3831,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -3833,7 +3844,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -3846,7 +3857,7 @@
       <c r="L88" s="8"/>
       <c r="M88" s="8"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -3859,7 +3870,7 @@
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -3874,12 +3885,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:F6"/>
-    <mergeCell ref="H5:M6"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -3892,6 +3897,12 @@
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:F6"/>
+    <mergeCell ref="H5:M6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A14:A17 H14:H17" xr:uid="{B48B5047-8C1F-4FFB-9FFA-F5906E31E514}">
@@ -3911,91 +3922,91 @@
       <selection activeCell="A8" sqref="A8:M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="66" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="35" customWidth="1"/>
-    <col min="14" max="16384" width="9.28515625" style="73"/>
+    <col min="1" max="1" width="3.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="66" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="35" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+    <row r="1" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-    </row>
-    <row r="2" spans="1:13" s="35" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+    </row>
+    <row r="2" spans="1:13" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="127"/>
-    </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+    </row>
+    <row r="3" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-    </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="126" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+    </row>
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-    </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+    </row>
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -4010,7 +4021,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -4025,61 +4036,61 @@
       <c r="L6" s="40"/>
       <c r="M6" s="41"/>
     </row>
-    <row r="7" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="128" t="s">
+    <row r="7" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="128"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
-    </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="130" t="s">
+      <c r="B7" s="135"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+    </row>
+    <row r="8" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="130" t="s">
+      <c r="B8" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="130" t="s">
+      <c r="C8" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="134" t="s">
+      <c r="D8" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="129" t="s">
+      <c r="E8" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="129" t="s">
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="130" t="s">
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="132" t="s">
+      <c r="L8" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="132" t="s">
+      <c r="M8" s="129" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="131"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="135"/>
+    <row r="9" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="128"/>
+      <c r="B9" s="128"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="43" t="s">
         <v>60</v>
       </c>
@@ -4098,11 +4109,11 @@
       <c r="J9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="131"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="132"/>
-    </row>
-    <row r="10" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="128"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
+    </row>
+    <row r="10" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>1</v>
       </c>
@@ -4144,7 +4155,7 @@
         <v>7410000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>2</v>
       </c>
@@ -4189,7 +4200,7 @@
         <v>24228000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>3</v>
       </c>
@@ -4234,7 +4245,7 @@
         <v>30013500</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>4</v>
       </c>
@@ -4280,7 +4291,7 @@
         <v>23313000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>5</v>
       </c>
@@ -4322,7 +4333,7 @@
         <v>10086000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>6</v>
       </c>
@@ -4366,7 +4377,7 @@
         <v>20649000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>7</v>
       </c>
@@ -4411,7 +4422,7 @@
         <v>18390000</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>8</v>
       </c>
@@ -4455,7 +4466,7 @@
         <v>10566000</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -4476,27 +4487,27 @@
         <v>144655500</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="133" t="s">
+    <row r="19" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="130" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="133"/>
-      <c r="C19" s="133"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133"/>
-      <c r="F19" s="133"/>
-      <c r="G19" s="133"/>
-      <c r="H19" s="133"/>
-      <c r="I19" s="133"/>
-      <c r="J19" s="133"/>
-      <c r="K19" s="133"/>
-      <c r="L19" s="133"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="130"/>
+      <c r="I19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130"/>
       <c r="M19" s="61">
         <f>M18/D18</f>
         <v>6027312.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="62"/>
       <c r="C20" s="62"/>
       <c r="D20" s="63"/>
@@ -4505,16 +4516,16 @@
       <c r="G20" s="64"/>
       <c r="M20" s="65"/>
     </row>
-    <row r="21" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="66"/>
       <c r="G21" s="67"/>
       <c r="M21" s="65"/>
     </row>
-    <row r="22" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="66"/>
       <c r="M22" s="65"/>
     </row>
-    <row r="23" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="68"/>
       <c r="C23" s="68"/>
       <c r="D23" s="69"/>
@@ -4525,7 +4536,7 @@
       <c r="L23" s="65"/>
       <c r="M23" s="65"/>
     </row>
-    <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="68"/>
       <c r="C24" s="68"/>
       <c r="D24" s="69"/>
@@ -4535,16 +4546,16 @@
       <c r="K24" s="65"/>
       <c r="M24" s="65"/>
     </row>
-    <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="66"/>
     </row>
-    <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="66"/>
       <c r="E26" s="70"/>
       <c r="F26" s="70"/>
       <c r="G26" s="70"/>
     </row>
-    <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="66"/>
       <c r="E27" s="70"/>
       <c r="F27" s="70"/>
@@ -4553,196 +4564,196 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="66"/>
       <c r="E28" s="70"/>
       <c r="F28" s="70"/>
       <c r="G28" s="70"/>
       <c r="J28" s="71"/>
     </row>
-    <row r="29" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="66"/>
       <c r="E29" s="70"/>
       <c r="F29" s="70"/>
       <c r="G29" s="70"/>
       <c r="J29" s="71"/>
     </row>
-    <row r="30" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="66"/>
       <c r="E30" s="70"/>
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
     </row>
-    <row r="31" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="66"/>
       <c r="E31" s="70"/>
       <c r="F31" s="70"/>
       <c r="G31" s="70"/>
     </row>
-    <row r="32" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="66"/>
       <c r="E32" s="70"/>
       <c r="F32" s="70"/>
       <c r="G32" s="70"/>
     </row>
-    <row r="33" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D33" s="66"/>
       <c r="E33" s="70"/>
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
     </row>
-    <row r="34" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D34" s="66"/>
       <c r="E34" s="70"/>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
     </row>
-    <row r="35" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="66"/>
       <c r="E35" s="70"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
       <c r="K35" s="68"/>
     </row>
-    <row r="36" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D36" s="66"/>
       <c r="E36" s="70"/>
       <c r="F36" s="70"/>
       <c r="G36" s="70"/>
     </row>
-    <row r="37" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D37" s="66"/>
       <c r="E37" s="70"/>
       <c r="F37" s="70"/>
       <c r="G37" s="70"/>
     </row>
-    <row r="38" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D38" s="66"/>
       <c r="E38" s="70"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
     </row>
-    <row r="39" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="66"/>
       <c r="E39" s="70"/>
       <c r="F39" s="70"/>
       <c r="G39" s="70"/>
     </row>
-    <row r="40" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D40" s="66"/>
       <c r="E40" s="70"/>
       <c r="F40" s="70"/>
       <c r="G40" s="70"/>
     </row>
-    <row r="41" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="66"/>
       <c r="E41" s="70"/>
       <c r="F41" s="70"/>
       <c r="G41" s="70"/>
     </row>
-    <row r="42" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="66"/>
     </row>
-    <row r="43" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="66"/>
     </row>
-    <row r="44" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="66"/>
     </row>
-    <row r="45" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D45" s="66"/>
     </row>
-    <row r="46" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D46" s="66"/>
     </row>
-    <row r="47" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D47" s="66"/>
     </row>
-    <row r="48" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" s="66"/>
     </row>
-    <row r="49" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" s="66"/>
     </row>
-    <row r="50" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" s="66"/>
     </row>
-    <row r="51" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="66"/>
     </row>
-    <row r="52" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="66"/>
     </row>
-    <row r="53" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="66"/>
     </row>
-    <row r="54" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="66"/>
     </row>
-    <row r="55" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="66"/>
     </row>
-    <row r="56" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="66"/>
     </row>
-    <row r="57" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="66"/>
     </row>
-    <row r="58" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="66"/>
     </row>
-    <row r="59" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="66"/>
     </row>
-    <row r="60" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="66"/>
     </row>
-    <row r="61" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="66"/>
     </row>
-    <row r="62" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="66"/>
     </row>
-    <row r="63" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="66"/>
     </row>
-    <row r="64" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="66"/>
     </row>
-    <row r="65" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="66"/>
     </row>
-    <row r="66" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" s="66"/>
     </row>
-    <row r="67" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" s="66"/>
     </row>
-    <row r="68" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" s="66"/>
     </row>
-    <row r="69" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D69" s="66"/>
     </row>
-    <row r="70" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D70" s="66"/>
     </row>
-    <row r="71" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D71" s="66"/>
     </row>
-    <row r="72" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D72" s="66"/>
     </row>
-    <row r="73" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D73" s="66"/>
     </row>
-    <row r="74" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D74" s="66"/>
     </row>
-    <row r="75" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" s="66"/>
     </row>
-    <row r="76" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
@@ -4759,6 +4770,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A7:M7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:L9"/>
@@ -4769,11 +4785,6 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:G8"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A7:M7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4788,78 +4799,78 @@
       <selection activeCell="N9" sqref="N9:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="66" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="35" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.28515625" style="73"/>
+    <col min="1" max="1" width="3.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="66" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.33203125" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="35" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+    <row r="1" spans="1:14" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="134" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-    </row>
-    <row r="2" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+    </row>
+    <row r="2" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-    </row>
-    <row r="3" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="126" t="s">
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="133"/>
+    </row>
+    <row r="3" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="126"/>
-    </row>
-    <row r="4" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+    </row>
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -4875,7 +4886,7 @@
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
     </row>
-    <row r="5" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="36"/>
       <c r="C5" s="37"/>
@@ -4891,36 +4902,36 @@
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
     </row>
-    <row r="6" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="128"/>
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-    </row>
-    <row r="7" spans="1:14" s="35" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="130" t="s">
+    <row r="6" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="135"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+    </row>
+    <row r="7" spans="1:14" s="35" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="130" t="s">
+      <c r="D7" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="134" t="s">
+      <c r="E7" s="131" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="136" t="s">
@@ -4928,27 +4939,27 @@
       </c>
       <c r="G7" s="136"/>
       <c r="H7" s="136"/>
-      <c r="I7" s="130" t="s">
+      <c r="I7" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="132" t="s">
+      <c r="J7" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="132" t="s">
+      <c r="K7" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="129" t="s">
+      <c r="L7" s="126" t="s">
         <v>85</v>
       </c>
-      <c r="M7" s="129"/>
-      <c r="N7" s="129"/>
-    </row>
-    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="131"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="135"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+    </row>
+    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="128"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="132"/>
       <c r="F8" s="43" t="s">
         <v>60</v>
       </c>
@@ -4958,9 +4969,9 @@
       <c r="H8" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="132"/>
-      <c r="K8" s="132"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
       <c r="L8" s="43" t="s">
         <v>60</v>
       </c>
@@ -4971,7 +4982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46">
         <v>1</v>
       </c>
@@ -5018,7 +5029,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>2</v>
       </c>
@@ -5063,7 +5074,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>3</v>
       </c>
@@ -5108,7 +5119,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>4</v>
       </c>
@@ -5153,7 +5164,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>5</v>
       </c>
@@ -5198,7 +5209,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>6</v>
       </c>
@@ -5243,7 +5254,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>7</v>
       </c>
@@ -5288,7 +5299,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>8</v>
       </c>
@@ -5331,7 +5342,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>9</v>
       </c>
@@ -5376,7 +5387,7 @@
         <v>11970000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>10</v>
       </c>
@@ -5421,7 +5432,7 @@
         <v>9576000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>11</v>
       </c>
@@ -5466,7 +5477,7 @@
         <v>19152000</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>12</v>
       </c>
@@ -5511,7 +5522,7 @@
         <v>16758000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46">
         <v>13</v>
       </c>
@@ -5556,7 +5567,7 @@
         <v>7182000</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
       <c r="B22" s="46"/>
       <c r="C22" s="47"/>
@@ -5581,7 +5592,7 @@
         <v>83790000</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="94" t="s">
         <v>69</v>
       </c>
@@ -5602,7 +5613,7 @@
       <c r="M23" s="94"/>
       <c r="N23" s="94"/>
     </row>
-    <row r="24" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="62"/>
       <c r="D24" s="62"/>
       <c r="E24" s="63"/>
@@ -5611,16 +5622,16 @@
       <c r="H24" s="64"/>
       <c r="K24" s="65"/>
     </row>
-    <row r="25" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E25" s="66"/>
       <c r="H25" s="67"/>
       <c r="K25" s="65"/>
     </row>
-    <row r="26" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E26" s="66"/>
       <c r="K26" s="65"/>
     </row>
-    <row r="27" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
       <c r="E27" s="69"/>
@@ -5631,7 +5642,7 @@
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
     </row>
-    <row r="28" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="68"/>
       <c r="D28" s="68"/>
       <c r="E28" s="69"/>
@@ -5641,16 +5652,16 @@
       <c r="I28" s="65"/>
       <c r="K28" s="65"/>
     </row>
-    <row r="29" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="66"/>
     </row>
-    <row r="30" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E30" s="66"/>
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
       <c r="H30" s="70"/>
     </row>
-    <row r="31" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E31" s="66"/>
       <c r="F31" s="70"/>
       <c r="G31" s="70"/>
@@ -5659,196 +5670,196 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E32" s="66"/>
       <c r="F32" s="70"/>
       <c r="G32" s="70"/>
       <c r="H32" s="70"/>
       <c r="N32" s="71"/>
     </row>
-    <row r="33" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E33" s="66"/>
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
       <c r="H33" s="70"/>
       <c r="N33" s="71"/>
     </row>
-    <row r="34" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E34" s="66"/>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
     </row>
-    <row r="35" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E35" s="66"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
       <c r="H35" s="70"/>
     </row>
-    <row r="36" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E36" s="66"/>
       <c r="F36" s="70"/>
       <c r="G36" s="70"/>
       <c r="H36" s="70"/>
     </row>
-    <row r="37" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E37" s="66"/>
       <c r="F37" s="70"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
     </row>
-    <row r="38" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E38" s="66"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
       <c r="H38" s="70"/>
     </row>
-    <row r="39" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E39" s="66"/>
       <c r="F39" s="70"/>
       <c r="G39" s="70"/>
       <c r="H39" s="70"/>
       <c r="I39" s="68"/>
     </row>
-    <row r="40" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E40" s="66"/>
       <c r="F40" s="70"/>
       <c r="G40" s="70"/>
       <c r="H40" s="70"/>
     </row>
-    <row r="41" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E41" s="66"/>
       <c r="F41" s="70"/>
       <c r="G41" s="70"/>
       <c r="H41" s="70"/>
     </row>
-    <row r="42" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E42" s="66"/>
       <c r="F42" s="70"/>
       <c r="G42" s="70"/>
       <c r="H42" s="70"/>
     </row>
-    <row r="43" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="66"/>
       <c r="F43" s="70"/>
       <c r="G43" s="70"/>
       <c r="H43" s="70"/>
     </row>
-    <row r="44" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E44" s="66"/>
       <c r="F44" s="70"/>
       <c r="G44" s="70"/>
       <c r="H44" s="70"/>
     </row>
-    <row r="45" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E45" s="66"/>
       <c r="F45" s="70"/>
       <c r="G45" s="70"/>
       <c r="H45" s="70"/>
     </row>
-    <row r="46" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E46" s="66"/>
     </row>
-    <row r="47" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="66"/>
     </row>
-    <row r="48" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E48" s="66"/>
     </row>
-    <row r="49" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E49" s="66"/>
     </row>
-    <row r="50" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="66"/>
     </row>
-    <row r="51" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E51" s="66"/>
     </row>
-    <row r="52" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="66"/>
     </row>
-    <row r="53" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E53" s="66"/>
     </row>
-    <row r="54" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E54" s="66"/>
     </row>
-    <row r="55" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="66"/>
     </row>
-    <row r="56" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E56" s="66"/>
     </row>
-    <row r="57" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E57" s="66"/>
     </row>
-    <row r="58" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E58" s="66"/>
     </row>
-    <row r="59" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E59" s="66"/>
     </row>
-    <row r="60" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E60" s="66"/>
     </row>
-    <row r="61" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E61" s="66"/>
     </row>
-    <row r="62" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E62" s="66"/>
     </row>
-    <row r="63" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E63" s="66"/>
     </row>
-    <row r="64" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E64" s="66"/>
     </row>
-    <row r="65" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E65" s="66"/>
     </row>
-    <row r="66" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E66" s="66"/>
     </row>
-    <row r="67" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E67" s="66"/>
     </row>
-    <row r="68" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E68" s="66"/>
     </row>
-    <row r="69" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E69" s="66"/>
     </row>
-    <row r="70" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E70" s="66"/>
     </row>
-    <row r="71" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E71" s="66"/>
     </row>
-    <row r="72" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E72" s="66"/>
     </row>
-    <row r="73" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E73" s="66"/>
     </row>
-    <row r="74" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E74" s="66"/>
     </row>
-    <row r="75" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E75" s="66"/>
     </row>
-    <row r="76" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E76" s="66"/>
     </row>
-    <row r="77" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E77" s="66"/>
     </row>
-    <row r="78" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E78" s="66"/>
     </row>
-    <row r="79" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E79" s="66"/>
     </row>
-    <row r="80" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="35"/>
       <c r="C80" s="35"/>
@@ -5894,19 +5905,19 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="108" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -5917,7 +5928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -5932,7 +5943,7 @@
         <v>19572000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -5950,7 +5961,7 @@
         <v>27000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -5968,7 +5979,7 @@
         <v>3840000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -5983,7 +5994,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" s="107">
         <f>SUM(E4:E7)</f>
         <v>53412000</v>

</xml_diff>